<commit_message>
Add the invisible task for new Algorithm
</commit_message>
<xml_diff>
--- a/DisorderEvent/file/result.xlsx
+++ b/DisorderEvent/file/result.xlsx
@@ -153,7 +153,7 @@
   <dimension ref="A1:C31"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
+      <selection pane="topLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -419,6 +419,9 @@
       <c r="A27" s="0" t="n">
         <v>1</v>
       </c>
+      <c r="B27" s="0" t="n">
+        <v>37</v>
+      </c>
       <c r="C27" s="0" t="n">
         <v>100</v>
       </c>

</xml_diff>

<commit_message>
add the new cost function
</commit_message>
<xml_diff>
--- a/DisorderEvent/file/result.xlsx
+++ b/DisorderEvent/file/result.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="196" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
   <si>
     <t>Alignment_Astar</t>
   </si>
@@ -33,6 +33,9 @@
     <t>simpara</t>
   </si>
   <si>
+    <t>=</t>
+  </si>
+  <si>
     <t>shortloop3</t>
   </si>
   <si>
@@ -46,6 +49,27 @@
   </si>
   <si>
     <t>shortloop3_rev</t>
+  </si>
+  <si>
+    <t>并发节点个数</t>
+  </si>
+  <si>
+    <t>只选１个</t>
+  </si>
+  <si>
+    <t>估价函数</t>
+  </si>
+  <si>
+    <t>针对并发</t>
+  </si>
+  <si>
+    <t>日志错的/对的</t>
+  </si>
+  <si>
+    <t>正确率</t>
+  </si>
+  <si>
+    <t>剪枝优化</t>
   </si>
   <si>
     <t>NewAlgorithm</t>
@@ -212,10 +236,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E50"/>
+  <dimension ref="A1:G55"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A11" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B46" activeCellId="0" sqref="B46"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A24" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B53" activeCellId="0" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
@@ -384,11 +408,18 @@
       <c r="E13" s="2" t="n">
         <v>1122</v>
       </c>
+      <c r="G13" s="0" t="e">
+        <f aca="false">10!</f>
+        <v>#N/A</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>4</v>
       </c>
+      <c r="G14" s="0" t="s">
+        <v>5</v>
+      </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
@@ -462,7 +493,7 @@
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -537,7 +568,7 @@
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -612,7 +643,7 @@
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -672,7 +703,7 @@
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -732,7 +763,7 @@
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -788,6 +819,35 @@
       </c>
       <c r="E50" s="2" t="n">
         <v>3325</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="s">
+        <v>17</v>
       </c>
     </row>
   </sheetData>
@@ -808,13 +868,15 @@
   </sheetPr>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="11.639175257732"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="0" width="23.159793814433"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="0" width="19.3659793814433"/>
+    <col collapsed="false" hidden="false" max="1025" min="3" style="0" width="11.639175257732"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -822,51 +884,51 @@
         <v>0</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>10</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>11</v>
+        <v>19</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>14</v>
+        <v>22</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>15</v>
+        <v>23</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>17</v>
+        <v>25</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>